<commit_message>
Updated Style Sheet spreadsheet document.
</commit_message>
<xml_diff>
--- a/MapboxStyleSheetSupport.xlsx
+++ b/MapboxStyleSheetSupport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjg/dev/WhirlyGlobe-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD06AC2-8B66-7448-A51C-0044CBCAA23C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42997806-BBEE-6649-BC2D-B7715B7BFD33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="16480" windowWidth="20320" windowHeight="16780" xr2:uid="{A8CB525C-51A5-C149-A19C-6A2CBD5E0523}"/>
+    <workbookView xWindow="33460" yWindow="1760" windowWidth="28640" windowHeight="23620" xr2:uid="{A8CB525C-51A5-C149-A19C-6A2CBD5E0523}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="88">
   <si>
     <t>Layer</t>
   </si>
@@ -156,9 +156,6 @@
     <t>text-font</t>
   </si>
   <si>
-    <t>Font names don't map well to iOS names</t>
-  </si>
-  <si>
     <t>text-max-width</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>stops</t>
   </si>
   <si>
-    <t>This causes problems with expressions that run through a lot of levels (4 through 20).</t>
-  </si>
-  <si>
     <t>Filters</t>
   </si>
   <si>
@@ -258,10 +252,43 @@
     <t>Functions</t>
   </si>
   <si>
-    <t>Functions work for double values and color values and assume a non-linear function.</t>
-  </si>
-  <si>
-    <t>All functions are evaluated statically at a given zoom level.</t>
+    <t>Continuous</t>
+  </si>
+  <si>
+    <t>Fonts have to be present in the app</t>
+  </si>
+  <si>
+    <t>fill-extrusion-color</t>
+  </si>
+  <si>
+    <t>fill-extrusion-opacity</t>
+  </si>
+  <si>
+    <t>Turning this into regular fill</t>
+  </si>
+  <si>
+    <t>Not handling this at all (sort of)</t>
+  </si>
+  <si>
+    <t>text-halo-blur</t>
+  </si>
+  <si>
+    <t>Blur is not quite right</t>
+  </si>
+  <si>
+    <t>Halos are different from our outlines</t>
+  </si>
+  <si>
+    <t>text-allow-overlap</t>
+  </si>
+  <si>
+    <t>icon-allow-overlap</t>
+  </si>
+  <si>
+    <t>text-justify</t>
+  </si>
+  <si>
+    <t>We only implement the old style of expressions for some text, most colors and doubles</t>
   </si>
 </sst>
 </file>
@@ -623,20 +650,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88258E4E-1616-5F44-ADBA-4823D4755AB6}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="6" max="6" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,8 +673,11 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -660,16 +690,22 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -680,50 +716,68 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -736,391 +790,490 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>19</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>20</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>30</v>
       </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
         <v>23</v>
       </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
         <v>24</v>
       </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>8</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>25</v>
       </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
         <v>26</v>
       </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
         <v>27</v>
       </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
         <v>28</v>
       </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>29</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>31</v>
       </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
         <v>32</v>
       </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
         <v>33</v>
       </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
         <v>34</v>
       </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="F34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>3</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>38</v>
       </c>
-      <c r="D34" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
         <v>39</v>
       </c>
-      <c r="D35" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
         <v>40</v>
       </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
         <v>42</v>
       </c>
-      <c r="D37" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
         <v>44</v>
       </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C39" t="s">
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
         <v>45</v>
       </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
         <v>46</v>
       </c>
-      <c r="D40" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C41" t="s">
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" t="s">
         <v>47</v>
       </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" t="s">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C42" t="s">
+      <c r="D47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
         <v>49</v>
       </c>
-      <c r="D42" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
         <v>50</v>
       </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C45" t="s">
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
         <v>51</v>
       </c>
-      <c r="D45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C46" t="s">
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
         <v>52</v>
       </c>
-      <c r="D46" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C47" t="s">
+      <c r="D52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" t="s">
         <v>53</v>
       </c>
-      <c r="D47" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
         <v>54</v>
       </c>
-      <c r="D49" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>76</v>
-      </c>
-      <c r="B51" t="s">
-        <v>2</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="F57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C52" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+      <c r="B61" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="C61" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B57" t="s">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C62" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C57" s="2" t="s">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C63" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C58" s="2" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C64" s="2" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C59" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C60" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C61" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C62" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C63" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C64" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C65" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C66" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C67" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C68" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C69" s="2"/>
+      <c r="C69" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
-        <v>72</v>
-      </c>
       <c r="C70" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C71" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C72" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>70</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C75" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C76" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>